<commit_message>
Add baseline and anomaly calculation guidelines to documentation
</commit_message>
<xml_diff>
--- a/alma/Объединенная_таблица.xlsx
+++ b/alma/Объединенная_таблица.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ruslan_safaev\alma_servie\alma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1DC8B2-33FB-4DB1-99A7-2DCC7A7AAA46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378A7986-1BA8-4AD9-BB82-362CC5010F55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Объединенные данные" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -245,7 +246,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,12 +263,6 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor rgb="FF4472C4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -298,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -318,13 +313,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -630,7 +622,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -857,14 +849,14 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" s="8" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="5">
         <v>48361</v>
       </c>
       <c r="D9" s="7" t="s">

</xml_diff>